<commit_message>
ajouts de la liste des composant (en cour)
</commit_message>
<xml_diff>
--- a/ressources/pages et accès.xlsx
+++ b/ressources/pages et accès.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\julie\OneDrive\Bureau\projet\A4\Projet Elective\Projet-Logiciel\ressources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A1DACF9D-548D-4A13-808A-C0A16B7024A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0404D676-EFAE-40C7-A4E2-BF0D2B663AD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{03F934A2-E78B-4049-B42C-C1CB2E47AC86}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="69">
   <si>
     <t>Utilisateurs</t>
   </si>
@@ -157,6 +157,81 @@
   </si>
   <si>
     <t>Recherche</t>
+  </si>
+  <si>
+    <t>Composant :</t>
+  </si>
+  <si>
+    <t>CreateOrder</t>
+  </si>
+  <si>
+    <t>Order</t>
+  </si>
+  <si>
+    <t>EditOrder</t>
+  </si>
+  <si>
+    <t>DeletOrder</t>
+  </si>
+  <si>
+    <t>PayOrder</t>
+  </si>
+  <si>
+    <t>Bouton</t>
+  </si>
+  <si>
+    <t>Prix</t>
+  </si>
+  <si>
+    <t>Client</t>
+  </si>
+  <si>
+    <t>Adresse</t>
+  </si>
+  <si>
+    <t>Texte</t>
+  </si>
+  <si>
+    <t>Champ</t>
+  </si>
+  <si>
+    <t>Account</t>
+  </si>
+  <si>
+    <t>ValidOrder</t>
+  </si>
+  <si>
+    <t>SeeAccount</t>
+  </si>
+  <si>
+    <t>CreateAccount</t>
+  </si>
+  <si>
+    <t>EditAccount</t>
+  </si>
+  <si>
+    <t>DeletAccount</t>
+  </si>
+  <si>
+    <t>SupsendAccount</t>
+  </si>
+  <si>
+    <t>Nom du compte</t>
+  </si>
+  <si>
+    <t>Role</t>
+  </si>
+  <si>
+    <t>Mail</t>
+  </si>
+  <si>
+    <t>nom du compte</t>
+  </si>
+  <si>
+    <t>MDP</t>
+  </si>
+  <si>
+    <t>Confirmer MDP</t>
   </si>
 </sst>
 </file>
@@ -172,12 +247,30 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -192,8 +285,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -508,10 +605,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A48C066A-23A5-4B8A-925D-8E30AF7855A7}">
-  <dimension ref="A1:H16"/>
+  <dimension ref="A1:H36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -750,6 +847,208 @@
         <v>41</v>
       </c>
     </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>44</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>46</v>
+      </c>
+      <c r="B22" t="s">
+        <v>58</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B23" t="s">
+        <v>45</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F23" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="G23" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B24" t="s">
+        <v>47</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F24" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="G24" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B25" t="s">
+        <v>48</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F25" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="G25" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B26" t="s">
+        <v>49</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F26" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="G26" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B27" t="s">
+        <v>57</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F27" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="G27" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>56</v>
+      </c>
+      <c r="B32" t="s">
+        <v>58</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="F32" s="4"/>
+    </row>
+    <row r="33" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B33" t="s">
+        <v>59</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="E33" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="F33" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="G33" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="34" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B34" t="s">
+        <v>60</v>
+      </c>
+      <c r="C34" s="4"/>
+      <c r="D34" s="4"/>
+      <c r="E34" s="4"/>
+      <c r="F34" s="4"/>
+      <c r="G34" s="4"/>
+    </row>
+    <row r="35" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B35" t="s">
+        <v>61</v>
+      </c>
+      <c r="C35" s="4"/>
+      <c r="D35" s="4"/>
+      <c r="E35" s="4"/>
+      <c r="F35" s="4"/>
+      <c r="G35" s="4"/>
+    </row>
+    <row r="36" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B36" t="s">
+        <v>62</v>
+      </c>
+      <c r="C36" s="4"/>
+      <c r="D36" s="4"/>
+      <c r="E36" s="4"/>
+      <c r="F36" s="4"/>
+      <c r="G36" s="4"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
début création des pages
</commit_message>
<xml_diff>
--- a/ressources/pages et accès.xlsx
+++ b/ressources/pages et accès.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\julie\OneDrive\Bureau\projet\A4\Projet Elective\Projet-Logiciel\ressources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0404D676-EFAE-40C7-A4E2-BF0D2B663AD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A4AE78F-3AE8-4752-97C1-D390352756F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{03F934A2-E78B-4049-B42C-C1CB2E47AC86}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="98">
   <si>
     <t>Utilisateurs</t>
   </si>
@@ -232,6 +232,93 @@
   </si>
   <si>
     <t>Confirmer MDP</t>
+  </si>
+  <si>
+    <t>OrderHistory</t>
+  </si>
+  <si>
+    <t>SeeOrderHistory</t>
+  </si>
+  <si>
+    <t>EditOrderHistory</t>
+  </si>
+  <si>
+    <t>Delivery</t>
+  </si>
+  <si>
+    <t>SeeDelivery</t>
+  </si>
+  <si>
+    <t>AcepteDelivery</t>
+  </si>
+  <si>
+    <t>ValidateDelivery</t>
+  </si>
+  <si>
+    <t>livreur</t>
+  </si>
+  <si>
+    <t>adresseClient</t>
+  </si>
+  <si>
+    <t>AdresseRestaurant</t>
+  </si>
+  <si>
+    <t>seeSponsorship</t>
+  </si>
+  <si>
+    <t>parain</t>
+  </si>
+  <si>
+    <t>Sponsorship (?)</t>
+  </si>
+  <si>
+    <t>Notification (?)</t>
+  </si>
+  <si>
+    <t>seeNotification</t>
+  </si>
+  <si>
+    <t>Item</t>
+  </si>
+  <si>
+    <t>CreateItem</t>
+  </si>
+  <si>
+    <t>SeeItem</t>
+  </si>
+  <si>
+    <t>EditItem</t>
+  </si>
+  <si>
+    <t>infoArticle</t>
+  </si>
+  <si>
+    <t>SeeMenu</t>
+  </si>
+  <si>
+    <t>CreateMenu</t>
+  </si>
+  <si>
+    <t>EditMenu</t>
+  </si>
+  <si>
+    <t>Statistiques</t>
+  </si>
+  <si>
+    <t>seeStatistiques</t>
+  </si>
+  <si>
+    <t>Dashboard</t>
+  </si>
+  <si>
+    <t>seeDashboard</t>
+  </si>
+  <si>
+    <t>seelogs</t>
+  </si>
+  <si>
+    <t>Etat (timeline)</t>
   </si>
 </sst>
 </file>
@@ -247,7 +334,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -272,6 +359,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -285,12 +378,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -605,10 +699,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A48C066A-23A5-4B8A-925D-8E30AF7855A7}">
-  <dimension ref="A1:H36"/>
+  <dimension ref="A1:H54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="C45" sqref="C45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -847,7 +941,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>44</v>
       </c>
@@ -861,7 +955,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>46</v>
       </c>
@@ -881,7 +975,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
         <v>45</v>
       </c>
@@ -901,7 +995,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B24" t="s">
         <v>47</v>
       </c>
@@ -921,75 +1015,136 @@
         <v>53</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B25" t="s">
         <v>48</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D25" s="3" t="s">
+      <c r="D25" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="E25" s="3" t="s">
+      <c r="E25" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F25" s="3" t="s">
+      <c r="F25" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="G25" s="3" t="s">
+      <c r="G25" s="1" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B26" t="s">
         <v>49</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D26" s="3" t="s">
+      <c r="D26" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="E26" s="3" t="s">
+      <c r="E26" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F26" s="3" t="s">
+      <c r="F26" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="G26" s="3" t="s">
+      <c r="G26" s="1" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B27" t="s">
         <v>57</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D27" s="3" t="s">
+      <c r="D27" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="E27" s="3" t="s">
+      <c r="E27" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F27" s="3" t="s">
+      <c r="F27" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="G27" s="3" t="s">
+      <c r="G27" s="1" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
         <v>56</v>
       </c>
+      <c r="B29" t="s">
+        <v>58</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="F29" s="4"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B30" t="s">
+        <v>59</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="F30" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="G30" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="H30" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B31" t="s">
+        <v>60</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="E31" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="F31" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="G31" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="H31" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B32" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="D32" s="1" t="s">
         <v>65</v>
@@ -997,57 +1152,275 @@
       <c r="E32" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="F32" s="4"/>
-    </row>
-    <row r="33" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="F32" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="H32" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B33" t="s">
-        <v>59</v>
-      </c>
-      <c r="C33" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C33" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="D33" s="3" t="s">
+      <c r="D33" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="E33" s="3" t="s">
+      <c r="E33" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="F33" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="F33" s="3" t="s">
+      <c r="G33" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="G33" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="34" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B34" t="s">
-        <v>60</v>
-      </c>
-      <c r="C34" s="4"/>
-      <c r="D34" s="4"/>
-      <c r="E34" s="4"/>
-      <c r="F34" s="4"/>
-      <c r="G34" s="4"/>
-    </row>
-    <row r="35" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="H33" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>69</v>
+      </c>
       <c r="B35" t="s">
-        <v>61</v>
-      </c>
-      <c r="C35" s="4"/>
-      <c r="D35" s="4"/>
-      <c r="E35" s="4"/>
-      <c r="F35" s="4"/>
-      <c r="G35" s="4"/>
-    </row>
-    <row r="36" spans="2:7" x14ac:dyDescent="0.3">
+        <v>70</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="G35" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B36" t="s">
-        <v>62</v>
-      </c>
-      <c r="C36" s="4"/>
-      <c r="D36" s="4"/>
-      <c r="E36" s="4"/>
-      <c r="F36" s="4"/>
-      <c r="G36" s="4"/>
+        <v>71</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D36" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="E36" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F36" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="G36" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>72</v>
+      </c>
+      <c r="B38" t="s">
+        <v>73</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="G38" s="5" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B39" t="s">
+        <v>74</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="F39" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B40" t="s">
+        <v>75</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="F40" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>84</v>
+      </c>
+      <c r="B42" t="s">
+        <v>86</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B43" t="s">
+        <v>85</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D43" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="E43" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="F43" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B44" t="s">
+        <v>87</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D44" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="E44" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="F44" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>15</v>
+      </c>
+      <c r="B46" t="s">
+        <v>89</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E46" s="4"/>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B47" t="s">
+        <v>90</v>
+      </c>
+      <c r="C47" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D47" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="E47" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B48" t="s">
+        <v>91</v>
+      </c>
+      <c r="C48" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D48" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="E48" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>81</v>
+      </c>
+      <c r="B50" t="s">
+        <v>79</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>82</v>
+      </c>
+      <c r="B51" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>92</v>
+      </c>
+      <c r="B52" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>94</v>
+      </c>
+      <c r="B53" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>38</v>
+      </c>
+      <c r="B54" t="s">
+        <v>96</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
suppretion de front_end_elective en vue V3
</commit_message>
<xml_diff>
--- a/ressources/pages et accès.xlsx
+++ b/ressources/pages et accès.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\julie\OneDrive\Bureau\projet\A4\Projet Elective\Projet-Logiciel\ressources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A4AE78F-3AE8-4752-97C1-D390352756F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB18DDB3-6147-4373-866A-67D9C0EAF4E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{03F934A2-E78B-4049-B42C-C1CB2E47AC86}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="99">
   <si>
     <t>Utilisateurs</t>
   </si>
@@ -187,6 +187,9 @@
   </si>
   <si>
     <t>Adresse</t>
+  </si>
+  <si>
+    <t>SeeOrder</t>
   </si>
   <si>
     <t>Texte</t>
@@ -701,8 +704,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A48C066A-23A5-4B8A-925D-8E30AF7855A7}">
   <dimension ref="A1:H54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="C45" sqref="C45"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -946,13 +949,13 @@
         <v>44</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>50</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.3">
@@ -960,7 +963,7 @@
         <v>46</v>
       </c>
       <c r="B22" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>52</v>
@@ -1057,7 +1060,7 @@
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B27" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>21</v>
@@ -1077,40 +1080,40 @@
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B29" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D29" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E29" s="1" t="s">
         <v>65</v>
-      </c>
-      <c r="E29" s="1" t="s">
-        <v>64</v>
       </c>
       <c r="F29" s="4"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B30" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C30" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="D30" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="D30" s="3" t="s">
+      <c r="E30" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="E30" s="3" t="s">
-        <v>64</v>
-      </c>
       <c r="F30" s="3" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="G30" s="3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="H30" s="2" t="s">
         <v>21</v>
@@ -1118,22 +1121,22 @@
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B31" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C31" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="D31" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="D31" s="3" t="s">
+      <c r="E31" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="E31" s="3" t="s">
-        <v>64</v>
-      </c>
       <c r="F31" s="3" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="H31" s="2" t="s">
         <v>21</v>
@@ -1141,22 +1144,22 @@
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B32" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C32" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D32" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="D32" s="1" t="s">
+      <c r="E32" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="E32" s="1" t="s">
-        <v>64</v>
-      </c>
       <c r="F32" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="H32" s="2" t="s">
         <v>21</v>
@@ -1164,22 +1167,22 @@
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B33" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C33" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D33" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="D33" s="1" t="s">
+      <c r="E33" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="E33" s="1" t="s">
-        <v>64</v>
-      </c>
       <c r="F33" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="H33" s="2" t="s">
         <v>21</v>
@@ -1187,10 +1190,10 @@
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B35" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D35" s="1" t="s">
         <v>52</v>
@@ -1207,7 +1210,7 @@
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B36" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C36" s="2" t="s">
         <v>21</v>
@@ -1227,39 +1230,39 @@
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B38" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>52</v>
       </c>
       <c r="D38" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="E38" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="E38" s="1" t="s">
-        <v>76</v>
-      </c>
       <c r="F38" s="1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="G38" s="5" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B39" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C39" s="1" t="s">
         <v>52</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="F39" s="2" t="s">
         <v>21</v>
@@ -1267,16 +1270,16 @@
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B40" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>52</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="F40" s="2" t="s">
         <v>21</v>
@@ -1284,10 +1287,10 @@
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B42" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C42" s="1" t="s">
         <v>12</v>
@@ -1296,12 +1299,12 @@
         <v>51</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B43" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C43" s="3" t="s">
         <v>12</v>
@@ -1310,7 +1313,7 @@
         <v>51</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="F43" s="2" t="s">
         <v>21</v>
@@ -1318,7 +1321,7 @@
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B44" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C44" s="3" t="s">
         <v>12</v>
@@ -1327,7 +1330,7 @@
         <v>51</v>
       </c>
       <c r="E44" s="3" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="F44" s="2" t="s">
         <v>21</v>
@@ -1338,7 +1341,7 @@
         <v>15</v>
       </c>
       <c r="B46" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C46" s="1" t="s">
         <v>15</v>
@@ -1350,7 +1353,7 @@
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B47" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C47" s="3" t="s">
         <v>15</v>
@@ -1364,7 +1367,7 @@
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B48" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C48" s="3" t="s">
         <v>15</v>
@@ -1378,40 +1381,40 @@
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B50" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C50" s="1" t="s">
         <v>52</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B51" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B52" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B53" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.3">
@@ -1419,10 +1422,11 @@
         <v>38</v>
       </c>
       <c r="B54" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>